<commit_message>
singletons still in the data, tried different approaches for wealth, PCs hexbins
</commit_message>
<xml_diff>
--- a/results/full_results.xlsx
+++ b/results/full_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Outcome</t>
   </si>
@@ -75,19 +75,10 @@
     <t xml:space="preserve">occupation</t>
   </si>
   <si>
-    <t xml:space="preserve">income_ind</t>
-  </si>
-  <si>
     <t xml:space="preserve">income_hh</t>
   </si>
   <si>
     <t xml:space="preserve">wealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">health_self</t>
-  </si>
-  <si>
-    <t xml:space="preserve">health_illness</t>
   </si>
   <si>
     <t xml:space="preserve">health_pc</t>
@@ -492,32 +483,32 @@
         <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>3.65873197888275</v>
+        <v>0.628403326389794</v>
       </c>
       <c r="D2" t="n">
-        <v>2.1782190027668</v>
+        <v>0.373611934001235</v>
       </c>
       <c r="E2" t="n">
-        <v>5.83695098164955</v>
+        <v>1.00201526039103</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2" t="n">
-        <v>0.373177539029328</v>
+        <v>0.37286052295794</v>
       </c>
       <c r="K2" t="n">
-        <v>0.321922577562015</v>
+        <v>0.321600410622503</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0246968211878793</v>
+        <v>0.016536344843651</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0537050860223734</v>
+        <v>0.0437600523208839</v>
       </c>
       <c r="N2" t="n">
-        <v>0.346619398749895</v>
+        <v>0.338136755466154</v>
       </c>
       <c r="O2"/>
     </row>
@@ -532,10 +523,10 @@
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3" t="n">
-        <v>3.4894121589811</v>
+        <v>0.601124756053185</v>
       </c>
       <c r="G3" t="n">
-        <v>1.87904630511576</v>
+        <v>0.322248519191769</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -559,10 +550,10 @@
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4" t="n">
-        <v>3.34525802430488</v>
+        <v>0.584555086168758</v>
       </c>
       <c r="I4" t="n">
-        <v>1.60949615460774</v>
+        <v>0.295148618358534</v>
       </c>
       <c r="J4"/>
       <c r="K4"/>
@@ -570,7 +561,7 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4" t="n">
-        <v>0.426882625051701</v>
+        <v>0.416620575278824</v>
       </c>
     </row>
     <row r="5">
@@ -581,32 +572,32 @@
         <v>16</v>
       </c>
       <c r="C5" t="n">
-        <v>44783.0192873919</v>
+        <v>0.840547924335136</v>
       </c>
       <c r="D5" t="n">
-        <v>9205.16110819903</v>
+        <v>0.158869024064627</v>
       </c>
       <c r="E5" t="n">
-        <v>53988.180395591</v>
+        <v>0.999416948399763</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5" t="n">
-        <v>0.170503266469614</v>
+        <v>0.158961706942236</v>
       </c>
       <c r="K5" t="n">
-        <v>0.15771563070601</v>
+        <v>0.147527867274261</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0226933264806369</v>
+        <v>0.00564194197276215</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0320559947644133</v>
+        <v>0.0149128932112853</v>
       </c>
       <c r="N5" t="n">
-        <v>0.180408957186647</v>
+        <v>0.153169809247023</v>
       </c>
       <c r="O5"/>
     </row>
@@ -621,10 +612,10 @@
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6" t="n">
-        <v>44277.5458631033</v>
+        <v>0.831282378539568</v>
       </c>
       <c r="G6" t="n">
-        <v>8514.77992176047</v>
+        <v>0.147441850915167</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -648,10 +639,10 @@
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="n">
-        <v>43052.3744592907</v>
+        <v>0.825643726110102</v>
       </c>
       <c r="I7" t="n">
-        <v>9297.426199587</v>
+        <v>0.144313053614388</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -659,7 +650,7 @@
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7" t="n">
-        <v>0.202559261234027</v>
+        <v>0.173874600153521</v>
       </c>
     </row>
     <row r="8">
@@ -670,32 +661,32 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>2121617852.45352</v>
+        <v>0.810272823295543</v>
       </c>
       <c r="D8" t="n">
-        <v>330933107.522388</v>
+        <v>0.192497530543022</v>
       </c>
       <c r="E8" t="n">
-        <v>2452550959.97591</v>
+        <v>1.00277035383857</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8" t="n">
-        <v>0.134934243130116</v>
+        <v>0.19196571758045</v>
       </c>
       <c r="K8" t="n">
-        <v>0.136567278671447</v>
+        <v>0.186480923757717</v>
       </c>
       <c r="L8" t="n">
-        <v>0.136214833259467</v>
+        <v>0.0415438838932949</v>
       </c>
       <c r="M8" t="n">
-        <v>0.148297441565192</v>
+        <v>0.0487501581564369</v>
       </c>
       <c r="N8" t="n">
-        <v>0.272782111930914</v>
+        <v>0.228024807651012</v>
       </c>
       <c r="O8"/>
     </row>
@@ -710,10 +701,10 @@
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9" t="n">
-        <v>2091984639.8543</v>
+        <v>0.803046585102834</v>
       </c>
       <c r="G9" t="n">
-        <v>334938210.406955</v>
+        <v>0.186997541900669</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -737,10 +728,10 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" t="n">
-        <v>1757910819.78084</v>
+        <v>0.761387609951326</v>
       </c>
       <c r="I10" t="n">
-        <v>243359695.550658</v>
+        <v>0.17528558879874</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
@@ -748,7 +739,7 @@
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10" t="n">
-        <v>0.283231684695308</v>
+        <v>0.240715875736887</v>
       </c>
     </row>
     <row r="11">
@@ -759,32 +750,32 @@
         <v>16</v>
       </c>
       <c r="C11" t="n">
-        <v>3767962171.5206</v>
+        <v>0.951016714391941</v>
       </c>
       <c r="D11" t="n">
-        <v>871266129.691704</v>
+        <v>0.0489091155884586</v>
       </c>
       <c r="E11" t="n">
-        <v>4639228301.21231</v>
+        <v>0.9999258299804</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11" t="n">
-        <v>0.187804107304663</v>
+        <v>0.0489127434475988</v>
       </c>
       <c r="K11" t="n">
-        <v>0.183181455986474</v>
+        <v>0.0474222712227744</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0683815131942404</v>
+        <v>0.0107625383293676</v>
       </c>
       <c r="M11" t="n">
-        <v>0.077090908526681</v>
+        <v>0.0125860520705872</v>
       </c>
       <c r="N11" t="n">
-        <v>0.251562969180714</v>
+        <v>0.058184809552142</v>
       </c>
       <c r="O11"/>
     </row>
@@ -799,10 +790,10 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12" t="n">
-        <v>3727557298.2079</v>
+        <v>0.949193335900772</v>
       </c>
       <c r="G12" t="n">
-        <v>849820594.869727</v>
+        <v>0.0474187539119884</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
@@ -826,10 +817,10 @@
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13" t="n">
-        <v>3410319846.91746</v>
+        <v>0.938431595829083</v>
       </c>
       <c r="I13" t="n">
-        <v>740878764.311249</v>
+        <v>0.0469716229368307</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -837,7 +828,7 @@
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13" t="n">
-        <v>0.264895015831344</v>
+        <v>0.061498795518186</v>
       </c>
     </row>
     <row r="14">
@@ -848,32 +839,32 @@
         <v>16</v>
       </c>
       <c r="C14" t="n">
-        <v>710264912737.077</v>
+        <v>0.864415353858616</v>
       </c>
       <c r="D14" t="n">
-        <v>143572231039.595</v>
+        <v>0.135543391803346</v>
       </c>
       <c r="E14" t="n">
-        <v>853837143776.672</v>
+        <v>0.999958745661963</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14"/>
       <c r="J14" t="n">
-        <v>0.16814943234321</v>
+        <v>0.135548983786944</v>
       </c>
       <c r="K14" t="n">
-        <v>0.162208193522877</v>
+        <v>0.119298745006146</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0515843789650267</v>
+        <v>0.0159878359068364</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0560196346318151</v>
+        <v>0.0154840978608468</v>
       </c>
       <c r="N14" t="n">
-        <v>0.213792572487904</v>
+        <v>0.135286580912982</v>
       </c>
       <c r="O14"/>
     </row>
@@ -888,10 +879,10 @@
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15" t="n">
-        <v>706477926706.627</v>
+        <v>0.864919071123226</v>
       </c>
       <c r="G15" t="n">
-        <v>138499380654.747</v>
+        <v>0.119293823415392</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -915,10 +906,10 @@
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16" t="n">
-        <v>662433267907.635</v>
+        <v>0.848931894783977</v>
       </c>
       <c r="I16" t="n">
-        <v>116730783392.741</v>
+        <v>0.130164535266283</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -926,274 +917,7 @@
       <c r="M16"/>
       <c r="N16"/>
       <c r="O16" t="n">
-        <v>0.224169066975025</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.237677422870191</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.0424420967215961</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.280119519591787</v>
-      </c>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17" t="n">
-        <v>0.151514242147231</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.14018310729212</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0.0136529440282604</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.0245050362414884</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0.15383605132038</v>
-      </c>
-      <c r="O17"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18" t="n">
-        <v>0.234637540012856</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.0392680246695526</v>
-      </c>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="O18"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19" t="n">
-        <v>0.230813083890646</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.0403776603474268</v>
-      </c>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19" t="n">
-        <v>0.17601927838872</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1.85547259483951</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.277161780237386</v>
-      </c>
-      <c r="E20" t="n">
-        <v>2.13263437507689</v>
-      </c>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20" t="n">
-        <v>0.129962164858846</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0.115839874271975</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0.0586744026265736</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0.0545481258394695</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0.174514276898549</v>
-      </c>
-      <c r="O20"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21" t="n">
-        <v>1.86427243455677</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.247044097877</v>
-      </c>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22" t="n">
-        <v>1.73914138657824</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0.276118885549136</v>
-      </c>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22" t="n">
-        <v>0.184510290698316</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.306433430888885</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.0484608898232826</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.354894320712167</v>
-      </c>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23" t="n">
-        <v>0.136550198171771</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0.120628850283813</v>
-      </c>
-      <c r="L23" t="n">
-        <v>0.0411392512307729</v>
-      </c>
-      <c r="M23" t="n">
-        <v>0.0411393522574129</v>
-      </c>
-      <c r="N23" t="n">
-        <v>0.161768101514586</v>
-      </c>
-      <c r="O23"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24" t="n">
-        <v>0.306433395035104</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.0428104938797635</v>
-      </c>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-      <c r="N24"/>
-      <c r="O24"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25" t="n">
-        <v>0.291833308414952</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0.0515704376740639</v>
-      </c>
-      <c r="J25"/>
-      <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
-      <c r="N25"/>
-      <c r="O25" t="n">
-        <v>0.177689550429184</v>
+        <v>0.151033081647791</v>
       </c>
     </row>
   </sheetData>
@@ -1212,16 +936,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -1232,13 +956,13 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.30101607720954</v>
+        <v>0.298202737443845</v>
       </c>
       <c r="C2" t="n">
-        <v>0.39222272029025</v>
+        <v>0.378070773488463</v>
       </c>
       <c r="D2" t="n">
-        <v>0.346619398749895</v>
+        <v>0.338136755466154</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -1249,13 +973,13 @@
         <v>14</v>
       </c>
       <c r="B3" t="n">
-        <v>0.393530609282941</v>
+        <v>0.382609287426784</v>
       </c>
       <c r="C3" t="n">
-        <v>0.460234640820462</v>
+        <v>0.450631863130863</v>
       </c>
       <c r="D3" t="n">
-        <v>0.426882625051701</v>
+        <v>0.416620575278824</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -1263,16 +987,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" t="n">
-        <v>0.333447924729169</v>
+        <v>0.337141214321999</v>
       </c>
       <c r="C4" t="n">
-        <v>0.412907153329487</v>
+        <v>0.408579831593881</v>
       </c>
       <c r="D4" t="n">
-        <v>0.373177539029328</v>
+        <v>0.37286052295794</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -1283,13 +1007,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>0.132663110581919</v>
+        <v>0.105670374593847</v>
       </c>
       <c r="C5" t="n">
-        <v>0.228154803791375</v>
+        <v>0.200669243900198</v>
       </c>
       <c r="D5" t="n">
-        <v>0.180408957186647</v>
+        <v>0.153169809247023</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -1300,13 +1024,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>0.15810601111875</v>
+        <v>0.130718990351118</v>
       </c>
       <c r="C6" t="n">
-        <v>0.247012511349304</v>
+        <v>0.217030209955925</v>
       </c>
       <c r="D6" t="n">
-        <v>0.202559261234027</v>
+        <v>0.173874600153521</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -1314,16 +1038,16 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" t="n">
-        <v>0.127194068656163</v>
+        <v>0.113028282697799</v>
       </c>
       <c r="C7" t="n">
-        <v>0.213812464283065</v>
+        <v>0.204895131186673</v>
       </c>
       <c r="D7" t="n">
-        <v>0.170503266469614</v>
+        <v>0.158961706942236</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -1334,13 +1058,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>0.21269817151018</v>
+        <v>0.16141670072646</v>
       </c>
       <c r="C8" t="n">
-        <v>0.332866052351649</v>
+        <v>0.294632914575565</v>
       </c>
       <c r="D8" t="n">
-        <v>0.272782111930914</v>
+        <v>0.228024807651012</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -1351,13 +1075,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>0.229764018917406</v>
+        <v>0.177579526448942</v>
       </c>
       <c r="C9" t="n">
-        <v>0.33669935047321</v>
+        <v>0.303852225024833</v>
       </c>
       <c r="D9" t="n">
-        <v>0.283231684695308</v>
+        <v>0.240715875736887</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
@@ -1365,16 +1089,16 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0391155529725255</v>
+        <v>0.118986693016939</v>
       </c>
       <c r="C10" t="n">
-        <v>0.230752933287706</v>
+        <v>0.264944742143962</v>
       </c>
       <c r="D10" t="n">
-        <v>0.134934243130116</v>
+        <v>0.19196571758045</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
@@ -1385,13 +1109,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.185028924807625</v>
+        <v>-0.171246722343432</v>
       </c>
       <c r="C11" t="n">
-        <v>0.318097013553804</v>
+        <v>0.287616341447716</v>
       </c>
       <c r="D11" t="n">
-        <v>0.251562969180714</v>
+        <v>0.058184809552142</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
@@ -1402,13 +1126,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.202794569891906</v>
+        <v>-0.162026001983956</v>
       </c>
       <c r="C12" t="n">
-        <v>0.326995461770782</v>
+        <v>0.285023593020328</v>
       </c>
       <c r="D12" t="n">
-        <v>0.264895015831344</v>
+        <v>0.061498795518186</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -1416,16 +1140,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0974293742073742</v>
+        <v>-0.183607030109368</v>
       </c>
       <c r="C13" t="n">
-        <v>0.278178840401951</v>
+        <v>0.281432517004566</v>
       </c>
       <c r="D13" t="n">
-        <v>0.187804107304663</v>
+        <v>0.0489127434475988</v>
       </c>
       <c r="E13" t="s">
         <v>21</v>
@@ -1436,13 +1160,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0882666281859442</v>
+        <v>0.0823570945728142</v>
       </c>
       <c r="C14" t="n">
-        <v>0.339318516789863</v>
+        <v>0.18821606725315</v>
       </c>
       <c r="D14" t="n">
-        <v>0.213792572487904</v>
+        <v>0.135286580912982</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
@@ -1453,13 +1177,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.101305341357599</v>
+        <v>0.103878965459785</v>
       </c>
       <c r="C15" t="n">
-        <v>0.347032792592452</v>
+        <v>0.198187197835797</v>
       </c>
       <c r="D15" t="n">
-        <v>0.224169066975025</v>
+        <v>0.151033081647791</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
@@ -1467,172 +1191,19 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.00216121015762524</v>
+        <v>0.0887154406906158</v>
       </c>
       <c r="C16" t="n">
-        <v>0.338460074844045</v>
+        <v>0.182382526883273</v>
       </c>
       <c r="D16" t="n">
-        <v>0.16814943234321</v>
+        <v>0.135548983786944</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0.108495074753112</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.199177027887648</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.15383605132038</v>
-      </c>
-      <c r="E17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0.133027845769927</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.219010711007512</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.17601927838872</v>
-      </c>
-      <c r="E18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="n">
-        <v>0.103140742194956</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.199887742099506</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.151514242147231</v>
-      </c>
-      <c r="E19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="n">
-        <v>0.119772505029129</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.229256048767968</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.174514276898549</v>
-      </c>
-      <c r="E20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0.134451127053458</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.234569454343173</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.184510290698316</v>
-      </c>
-      <c r="E21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="n">
-        <v>0.074817330043974</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.185106999673718</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.129962164858846</v>
-      </c>
-      <c r="E22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" t="n">
-        <v>0.107901330552447</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.215634872476724</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.161768101514586</v>
-      </c>
-      <c r="E23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="n">
-        <v>0.130432769437533</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.224946331420835</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.177689550429184</v>
-      </c>
-      <c r="E24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="n">
-        <v>0.0817796627904207</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.191320733553122</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.136550198171771</v>
-      </c>
-      <c r="E25" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recovered negative wealth values, added wealth 6, recoded all health variables, tried to build wealth variable from scratch
</commit_message>
<xml_diff>
--- a/results/full_results.xlsx
+++ b/results/full_results.xlsx
@@ -483,32 +483,32 @@
         <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.628403326389794</v>
+        <v>0.633801763604265</v>
       </c>
       <c r="D2" t="n">
-        <v>0.373611934001235</v>
+        <v>0.366430595843073</v>
       </c>
       <c r="E2" t="n">
-        <v>1.00201526039103</v>
+        <v>1.00023235944734</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2" t="n">
-        <v>0.37286052295794</v>
+        <v>0.366345472011661</v>
       </c>
       <c r="K2" t="n">
-        <v>0.321600410622503</v>
+        <v>0.320947599833706</v>
       </c>
       <c r="L2" t="n">
-        <v>0.016536344843651</v>
+        <v>0.018590980859496</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0437600523208839</v>
+        <v>0.0470251163823176</v>
       </c>
       <c r="N2" t="n">
-        <v>0.338136755466154</v>
+        <v>0.339538580693202</v>
       </c>
       <c r="O2"/>
     </row>
@@ -523,10 +523,10 @@
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3" t="n">
-        <v>0.601124756053185</v>
+        <v>0.605361021141428</v>
       </c>
       <c r="G3" t="n">
-        <v>0.322248519191769</v>
+        <v>0.321022175040627</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -550,10 +550,10 @@
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4" t="n">
-        <v>0.584555086168758</v>
+        <v>0.586765720491894</v>
       </c>
       <c r="I4" t="n">
-        <v>0.295148618358534</v>
+        <v>0.295325091261613</v>
       </c>
       <c r="J4"/>
       <c r="K4"/>
@@ -561,7 +561,7 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4" t="n">
-        <v>0.416620575278824</v>
+        <v>0.413370588393979</v>
       </c>
     </row>
     <row r="5">
@@ -572,32 +572,32 @@
         <v>16</v>
       </c>
       <c r="C5" t="n">
-        <v>0.840547924335136</v>
+        <v>0.742751878844297</v>
       </c>
       <c r="D5" t="n">
-        <v>0.158869024064627</v>
+        <v>0.257411349567696</v>
       </c>
       <c r="E5" t="n">
-        <v>0.999416948399763</v>
+        <v>1.00016322841199</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5" t="n">
-        <v>0.158961706942236</v>
+        <v>0.257369339579101</v>
       </c>
       <c r="K5" t="n">
-        <v>0.147527867274261</v>
+        <v>0.249812828091976</v>
       </c>
       <c r="L5" t="n">
-        <v>0.00564194197276215</v>
+        <v>0.0043189614498902</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0149128932112853</v>
+        <v>0.0234052462131984</v>
       </c>
       <c r="N5" t="n">
-        <v>0.153169809247023</v>
+        <v>0.254131789541866</v>
       </c>
       <c r="O5"/>
     </row>
@@ -612,10 +612,10 @@
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6" t="n">
-        <v>0.831282378539568</v>
+        <v>0.723662478657036</v>
       </c>
       <c r="G6" t="n">
-        <v>0.147441850915167</v>
+        <v>0.249853604643201</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -639,10 +639,10 @@
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="n">
-        <v>0.825643726110102</v>
+        <v>0.719342812229927</v>
       </c>
       <c r="I7" t="n">
-        <v>0.144313053614388</v>
+        <v>0.240688908400512</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -650,7 +650,7 @@
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7" t="n">
-        <v>0.173874600153521</v>
+        <v>0.280774585792299</v>
       </c>
     </row>
     <row r="8">
@@ -661,32 +661,32 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.810272823295543</v>
+        <v>0.826274115984803</v>
       </c>
       <c r="D8" t="n">
-        <v>0.192497530543022</v>
+        <v>0.17383611324454</v>
       </c>
       <c r="E8" t="n">
-        <v>1.00277035383857</v>
+        <v>1.00011022922934</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8" t="n">
-        <v>0.19196571758045</v>
+        <v>0.173816953535705</v>
       </c>
       <c r="K8" t="n">
-        <v>0.186480923757717</v>
+        <v>0.166889298996757</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0415438838932949</v>
+        <v>0.0452814718576168</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0487501581564369</v>
+        <v>0.0523481805095654</v>
       </c>
       <c r="N8" t="n">
-        <v>0.228024807651012</v>
+        <v>0.212170770854374</v>
       </c>
       <c r="O8"/>
     </row>
@@ -701,10 +701,10 @@
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9" t="n">
-        <v>0.803046585102834</v>
+        <v>0.819206628375006</v>
       </c>
       <c r="G9" t="n">
-        <v>0.186997541900669</v>
+        <v>0.166907695075571</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -728,10 +728,10 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" t="n">
-        <v>0.761387609951326</v>
+        <v>0.773920165175643</v>
       </c>
       <c r="I10" t="n">
-        <v>0.17528558879874</v>
+        <v>0.139955424415778</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
@@ -739,7 +739,7 @@
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10" t="n">
-        <v>0.240715875736887</v>
+        <v>0.22616513404527</v>
       </c>
     </row>
     <row r="11">
@@ -750,32 +750,32 @@
         <v>16</v>
       </c>
       <c r="C11" t="n">
-        <v>0.824802763049781</v>
+        <v>0.795487272157285</v>
       </c>
       <c r="D11" t="n">
-        <v>0.17514907679814</v>
+        <v>0.204642490406254</v>
       </c>
       <c r="E11" t="n">
-        <v>0.99995183984792</v>
+        <v>1.00012976256354</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11" t="n">
-        <v>0.175157512410575</v>
+        <v>0.204615938917479</v>
       </c>
       <c r="K11" t="n">
-        <v>0.169717630477593</v>
+        <v>0.200416297218675</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0131664936095722</v>
+        <v>0.0144642158193792</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0179997681824154</v>
+        <v>0.0165717325187064</v>
       </c>
       <c r="N11" t="n">
-        <v>0.182884124087165</v>
+        <v>0.214880513038054</v>
       </c>
       <c r="O11"/>
     </row>
@@ -790,10 +790,10 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12" t="n">
-        <v>0.819969721248176</v>
+        <v>0.793379481981188</v>
       </c>
       <c r="G12" t="n">
-        <v>0.169709456850698</v>
+        <v>0.200442303751177</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
@@ -817,10 +817,10 @@
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13" t="n">
-        <v>0.806803861738938</v>
+        <v>0.778913389248085</v>
       </c>
       <c r="I13" t="n">
-        <v>0.163745459836471</v>
+        <v>0.184867996968001</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -828,7 +828,7 @@
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13" t="n">
-        <v>0.193157280592991</v>
+        <v>0.221187671436185</v>
       </c>
     </row>
     <row r="14">
@@ -839,32 +839,32 @@
         <v>16</v>
       </c>
       <c r="C14" t="n">
-        <v>0.864415353858616</v>
+        <v>0.86250241446824</v>
       </c>
       <c r="D14" t="n">
-        <v>0.135543391803346</v>
+        <v>0.137584829876363</v>
       </c>
       <c r="E14" t="n">
-        <v>0.999958745661963</v>
+        <v>1.0000872443446</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14"/>
       <c r="J14" t="n">
-        <v>0.135548983786944</v>
+        <v>0.137572827425199</v>
       </c>
       <c r="K14" t="n">
-        <v>0.119298745006146</v>
+        <v>0.119234023054421</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0159878359068364</v>
+        <v>0.0167303538278092</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0154840978608468</v>
+        <v>0.0181539368432949</v>
       </c>
       <c r="N14" t="n">
-        <v>0.135286580912982</v>
+        <v>0.135964376882231</v>
       </c>
       <c r="O14"/>
     </row>
@@ -879,10 +879,10 @@
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15" t="n">
-        <v>0.864919071123226</v>
+        <v>0.861078707253187</v>
       </c>
       <c r="G15" t="n">
-        <v>0.119293823415392</v>
+        <v>0.119244425548617</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -906,10 +906,10 @@
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16" t="n">
-        <v>0.848931894783977</v>
+        <v>0.844346893796624</v>
       </c>
       <c r="I16" t="n">
-        <v>0.130164535266283</v>
+        <v>0.132889035732967</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -917,7 +917,7 @@
       <c r="M16"/>
       <c r="N16"/>
       <c r="O16" t="n">
-        <v>0.151033081647791</v>
+        <v>0.155726764268494</v>
       </c>
     </row>
   </sheetData>
@@ -956,13 +956,13 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.297940960551911</v>
+        <v>0.288450894757233</v>
       </c>
       <c r="C2" t="n">
-        <v>0.378332550380397</v>
+        <v>0.39062626662917</v>
       </c>
       <c r="D2" t="n">
-        <v>0.338136755466154</v>
+        <v>0.339538580693202</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -973,13 +973,13 @@
         <v>14</v>
       </c>
       <c r="B3" t="n">
-        <v>0.382315922210656</v>
+        <v>0.369799925502681</v>
       </c>
       <c r="C3" t="n">
-        <v>0.450925228346991</v>
+        <v>0.456941251285277</v>
       </c>
       <c r="D3" t="n">
-        <v>0.416620575278824</v>
+        <v>0.413370588393979</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -990,13 +990,13 @@
         <v>27</v>
       </c>
       <c r="B4" t="n">
-        <v>0.335335130912478</v>
+        <v>0.319321936255042</v>
       </c>
       <c r="C4" t="n">
-        <v>0.410385915003401</v>
+        <v>0.41336900776828</v>
       </c>
       <c r="D4" t="n">
-        <v>0.37286052295794</v>
+        <v>0.366345472011661</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -1007,13 +1007,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>0.109958012062905</v>
+        <v>0.204974770901499</v>
       </c>
       <c r="C5" t="n">
-        <v>0.196381606431141</v>
+        <v>0.303288808182232</v>
       </c>
       <c r="D5" t="n">
-        <v>0.153169809247023</v>
+        <v>0.254131789541866</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -1024,13 +1024,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>0.134405297257984</v>
+        <v>0.236990032243043</v>
       </c>
       <c r="C6" t="n">
-        <v>0.213343903049058</v>
+        <v>0.324559139341555</v>
       </c>
       <c r="D6" t="n">
-        <v>0.173874600153521</v>
+        <v>0.280774585792299</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -1041,13 +1041,13 @@
         <v>27</v>
       </c>
       <c r="B7" t="n">
-        <v>0.120604789482616</v>
+        <v>0.209991870675951</v>
       </c>
       <c r="C7" t="n">
-        <v>0.197318624401856</v>
+        <v>0.304746808482251</v>
       </c>
       <c r="D7" t="n">
-        <v>0.158961706942236</v>
+        <v>0.257369339579101</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -1058,13 +1058,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>0.153931751397568</v>
+        <v>0.0915492622240084</v>
       </c>
       <c r="C8" t="n">
-        <v>0.302117863904457</v>
+        <v>0.332792279484739</v>
       </c>
       <c r="D8" t="n">
-        <v>0.228024807651012</v>
+        <v>0.212170770854374</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -1075,13 +1075,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>0.170506637359144</v>
+        <v>0.117570375658827</v>
       </c>
       <c r="C9" t="n">
-        <v>0.31092511411463</v>
+        <v>0.334759892431713</v>
       </c>
       <c r="D9" t="n">
-        <v>0.240715875736887</v>
+        <v>0.22616513404527</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
@@ -1092,13 +1092,13 @@
         <v>27</v>
       </c>
       <c r="B10" t="n">
-        <v>0.112851750293891</v>
+        <v>0.049050412637938</v>
       </c>
       <c r="C10" t="n">
-        <v>0.27107968486701</v>
+        <v>0.298583494433472</v>
       </c>
       <c r="D10" t="n">
-        <v>0.19196571758045</v>
+        <v>0.173816953535705</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
@@ -1109,13 +1109,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.030223976819082</v>
+        <v>0.0654657339104391</v>
       </c>
       <c r="C11" t="n">
-        <v>0.335544271355248</v>
+        <v>0.36429529216567</v>
       </c>
       <c r="D11" t="n">
-        <v>0.182884124087165</v>
+        <v>0.214880513038054</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
@@ -1126,13 +1126,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0449753397859461</v>
+        <v>0.0836029492781559</v>
       </c>
       <c r="C12" t="n">
-        <v>0.341339221400035</v>
+        <v>0.358772393594215</v>
       </c>
       <c r="D12" t="n">
-        <v>0.193157280592991</v>
+        <v>0.221187671436185</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -1143,13 +1143,13 @@
         <v>27</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0178123200332775</v>
+        <v>0.0515766372614611</v>
       </c>
       <c r="C13" t="n">
-        <v>0.332502704787873</v>
+        <v>0.357655240573497</v>
       </c>
       <c r="D13" t="n">
-        <v>0.175157512410575</v>
+        <v>0.204615938917479</v>
       </c>
       <c r="E13" t="s">
         <v>21</v>
@@ -1160,13 +1160,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0837529360811731</v>
+        <v>0.0627571799624126</v>
       </c>
       <c r="C14" t="n">
-        <v>0.186820225744791</v>
+        <v>0.209171573802048</v>
       </c>
       <c r="D14" t="n">
-        <v>0.135286580912982</v>
+        <v>0.135964376882231</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
@@ -1177,13 +1177,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.103911337756036</v>
+        <v>0.0883313212345291</v>
       </c>
       <c r="C15" t="n">
-        <v>0.198154825539546</v>
+        <v>0.223122207302459</v>
       </c>
       <c r="D15" t="n">
-        <v>0.151033081647791</v>
+        <v>0.155726764268494</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
@@ -1194,13 +1194,13 @@
         <v>27</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0863288670363686</v>
+        <v>0.0678552224499854</v>
       </c>
       <c r="C16" t="n">
-        <v>0.18476910053752</v>
+        <v>0.207290432400413</v>
       </c>
       <c r="D16" t="n">
-        <v>0.135548983786944</v>
+        <v>0.137572827425199</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
changed OCCU variables, added set.seed to bootstrapping
</commit_message>
<xml_diff>
--- a/results/full_results.xlsx
+++ b/results/full_results.xlsx
@@ -483,32 +483,32 @@
         <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.633801763604265</v>
+        <v>0.646323325211804</v>
       </c>
       <c r="D2" t="n">
-        <v>0.366430595843073</v>
+        <v>0.353901374928943</v>
       </c>
       <c r="E2" t="n">
-        <v>1.00023235944734</v>
+        <v>1.00022470014075</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2" t="n">
-        <v>0.366345472011661</v>
+        <v>0.353821871104706</v>
       </c>
       <c r="K2" t="n">
-        <v>0.320947599833706</v>
+        <v>0.306030320695031</v>
       </c>
       <c r="L2" t="n">
-        <v>0.018590980859496</v>
+        <v>0.0140135097358763</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0470251163823176</v>
+        <v>0.044042949480424</v>
       </c>
       <c r="N2" t="n">
-        <v>0.339538580693202</v>
+        <v>0.320043830430907</v>
       </c>
       <c r="O2"/>
     </row>
@@ -523,10 +523,10 @@
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3" t="n">
-        <v>0.605361021141428</v>
+        <v>0.61628713784792</v>
       </c>
       <c r="G3" t="n">
-        <v>0.321022175040627</v>
+        <v>0.306099085751164</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -550,10 +550,10 @@
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4" t="n">
-        <v>0.586765720491894</v>
+        <v>0.602270479274433</v>
       </c>
       <c r="I4" t="n">
-        <v>0.295325091261613</v>
+        <v>0.285664744666187</v>
       </c>
       <c r="J4"/>
       <c r="K4"/>
@@ -561,7 +561,7 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4" t="n">
-        <v>0.413370588393979</v>
+        <v>0.39786482058513</v>
       </c>
     </row>
     <row r="5">
@@ -572,32 +572,32 @@
         <v>16</v>
       </c>
       <c r="C5" t="n">
-        <v>0.742751878844297</v>
+        <v>0.87736090521989</v>
       </c>
       <c r="D5" t="n">
-        <v>0.257411349567696</v>
+        <v>0.122717006372813</v>
       </c>
       <c r="E5" t="n">
-        <v>1.00016322841199</v>
+        <v>1.0000779115927</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5" t="n">
-        <v>0.257369339579101</v>
+        <v>0.122707446040255</v>
       </c>
       <c r="K5" t="n">
-        <v>0.249812828091976</v>
+        <v>0.124661493700764</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0043189614498902</v>
+        <v>0.0258778380079757</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0234052462131984</v>
+        <v>0.0575515385189966</v>
       </c>
       <c r="N5" t="n">
-        <v>0.254131789541866</v>
+        <v>0.15053933170874</v>
       </c>
       <c r="O5"/>
     </row>
@@ -612,10 +612,10 @@
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6" t="n">
-        <v>0.723662478657036</v>
+        <v>0.845684736960415</v>
       </c>
       <c r="G6" t="n">
-        <v>0.249853604643201</v>
+        <v>0.124671206276287</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -639,10 +639,10 @@
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="n">
-        <v>0.719342812229927</v>
+        <v>0.819804882768865</v>
       </c>
       <c r="I7" t="n">
-        <v>0.240688908400512</v>
+        <v>0.125102165595073</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -650,7 +650,7 @@
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7" t="n">
-        <v>0.280774585792299</v>
+        <v>0.180258984559252</v>
       </c>
     </row>
     <row r="8">
@@ -661,32 +661,32 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.826274115984803</v>
+        <v>0.835673869589237</v>
       </c>
       <c r="D8" t="n">
-        <v>0.17383611324454</v>
+        <v>0.164430530342826</v>
       </c>
       <c r="E8" t="n">
-        <v>1.00011022922934</v>
+        <v>1.00010439993206</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8" t="n">
-        <v>0.173816953535705</v>
+        <v>0.164413365598627</v>
       </c>
       <c r="K8" t="n">
-        <v>0.166889298996757</v>
+        <v>0.155149501851177</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0452814718576168</v>
+        <v>0.0418768879942465</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0523481805095654</v>
+        <v>0.0497546069970125</v>
       </c>
       <c r="N8" t="n">
-        <v>0.212170770854374</v>
+        <v>0.197026389845424</v>
       </c>
       <c r="O8"/>
     </row>
@@ -701,10 +701,10 @@
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9" t="n">
-        <v>0.819206628375006</v>
+        <v>0.827795328153142</v>
       </c>
       <c r="G9" t="n">
-        <v>0.166907695075571</v>
+        <v>0.15516569944863</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -728,10 +728,10 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" t="n">
-        <v>0.773920165175643</v>
+        <v>0.785914068214634</v>
       </c>
       <c r="I10" t="n">
-        <v>0.139955424415778</v>
+        <v>0.129262717242758</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
@@ -739,7 +739,7 @@
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10" t="n">
-        <v>0.22616513404527</v>
+        <v>0.21416797259564</v>
       </c>
     </row>
     <row r="11">
@@ -750,32 +750,32 @@
         <v>16</v>
       </c>
       <c r="C11" t="n">
-        <v>0.795487272157285</v>
+        <v>0.768779677316853</v>
       </c>
       <c r="D11" t="n">
-        <v>0.204642490406254</v>
+        <v>0.231367222074937</v>
       </c>
       <c r="E11" t="n">
-        <v>1.00012976256354</v>
+        <v>1.00014689939179</v>
       </c>
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11" t="n">
-        <v>0.204615938917479</v>
+        <v>0.231333239362774</v>
       </c>
       <c r="K11" t="n">
-        <v>0.200416297218675</v>
+        <v>0.225387262095531</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0144642158193792</v>
+        <v>0.0283411036012153</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0165717325187064</v>
+        <v>0.0328616107307432</v>
       </c>
       <c r="N11" t="n">
-        <v>0.214880513038054</v>
+        <v>0.253728365696746</v>
       </c>
       <c r="O11"/>
     </row>
@@ -790,10 +790,10 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12" t="n">
-        <v>0.793379481981188</v>
+        <v>0.764258506127577</v>
       </c>
       <c r="G12" t="n">
-        <v>0.200442303751177</v>
+        <v>0.22542037134725</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
@@ -817,10 +817,10 @@
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13" t="n">
-        <v>0.778913389248085</v>
+        <v>0.73591323923548</v>
       </c>
       <c r="I13" t="n">
-        <v>0.184867996968001</v>
+        <v>0.220052021730966</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -828,7 +828,7 @@
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13" t="n">
-        <v>0.221187671436185</v>
+        <v>0.264194850093517</v>
       </c>
     </row>
     <row r="14">
@@ -839,32 +839,32 @@
         <v>16</v>
       </c>
       <c r="C14" t="n">
-        <v>0.86250241446824</v>
+        <v>0.86056319164205</v>
       </c>
       <c r="D14" t="n">
-        <v>0.137584829876363</v>
+        <v>0.139525364609732</v>
       </c>
       <c r="E14" t="n">
-        <v>1.0000872443446</v>
+        <v>1.00008855625178</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14"/>
       <c r="J14" t="n">
-        <v>0.137572827425199</v>
+        <v>0.139513009860504</v>
       </c>
       <c r="K14" t="n">
-        <v>0.119234023054421</v>
+        <v>0.12889266239111</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0167303538278092</v>
+        <v>0.0156862351653176</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0181539368432949</v>
+        <v>0.0268614147365685</v>
       </c>
       <c r="N14" t="n">
-        <v>0.135964376882231</v>
+        <v>0.144578897556428</v>
       </c>
       <c r="O14"/>
     </row>
@@ -879,10 +879,10 @@
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15" t="n">
-        <v>0.861078707253187</v>
+        <v>0.849387022438783</v>
       </c>
       <c r="G15" t="n">
-        <v>0.119244425548617</v>
+        <v>0.128904076642174</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -906,10 +906,10 @@
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16" t="n">
-        <v>0.844346893796624</v>
+        <v>0.833699398159275</v>
       </c>
       <c r="I16" t="n">
-        <v>0.132889035732967</v>
+        <v>0.140850119093156</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -917,7 +917,7 @@
       <c r="M16"/>
       <c r="N16"/>
       <c r="O16" t="n">
-        <v>0.155726764268494</v>
+        <v>0.166374424597072</v>
       </c>
     </row>
   </sheetData>
@@ -956,13 +956,13 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.288450894757233</v>
+        <v>0.258402143126609</v>
       </c>
       <c r="C2" t="n">
-        <v>0.39062626662917</v>
+        <v>0.381685517735206</v>
       </c>
       <c r="D2" t="n">
-        <v>0.339538580693202</v>
+        <v>0.320043830430907</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -973,13 +973,13 @@
         <v>14</v>
       </c>
       <c r="B3" t="n">
-        <v>0.369799925502681</v>
+        <v>0.350235918909555</v>
       </c>
       <c r="C3" t="n">
-        <v>0.456941251285277</v>
+        <v>0.445493722260706</v>
       </c>
       <c r="D3" t="n">
-        <v>0.413370588393979</v>
+        <v>0.39786482058513</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -990,13 +990,13 @@
         <v>27</v>
       </c>
       <c r="B4" t="n">
-        <v>0.319321936255042</v>
+        <v>0.302156483748208</v>
       </c>
       <c r="C4" t="n">
-        <v>0.41336900776828</v>
+        <v>0.405487258461205</v>
       </c>
       <c r="D4" t="n">
-        <v>0.366345472011661</v>
+        <v>0.353821871104706</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -1007,13 +1007,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>0.204974770901499</v>
+        <v>0.0803137283705362</v>
       </c>
       <c r="C5" t="n">
-        <v>0.303288808182232</v>
+        <v>0.220764935046943</v>
       </c>
       <c r="D5" t="n">
-        <v>0.254131789541866</v>
+        <v>0.15053933170874</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -1024,13 +1024,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>0.236990032243043</v>
+        <v>0.118786280157073</v>
       </c>
       <c r="C6" t="n">
-        <v>0.324559139341555</v>
+        <v>0.241731688961431</v>
       </c>
       <c r="D6" t="n">
-        <v>0.280774585792299</v>
+        <v>0.180258984559252</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -1041,13 +1041,13 @@
         <v>27</v>
       </c>
       <c r="B7" t="n">
-        <v>0.209991870675951</v>
+        <v>0.0639261260280642</v>
       </c>
       <c r="C7" t="n">
-        <v>0.304746808482251</v>
+        <v>0.181488766052447</v>
       </c>
       <c r="D7" t="n">
-        <v>0.257369339579101</v>
+        <v>0.122707446040255</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -1058,13 +1058,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0915492622240084</v>
+        <v>0.0850071193212848</v>
       </c>
       <c r="C8" t="n">
-        <v>0.332792279484739</v>
+        <v>0.309045660369563</v>
       </c>
       <c r="D8" t="n">
-        <v>0.212170770854374</v>
+        <v>0.197026389845424</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -1075,13 +1075,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>0.117570375658827</v>
+        <v>0.110050467661553</v>
       </c>
       <c r="C9" t="n">
-        <v>0.334759892431713</v>
+        <v>0.318285477529726</v>
       </c>
       <c r="D9" t="n">
-        <v>0.22616513404527</v>
+        <v>0.21416797259564</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
@@ -1092,13 +1092,13 @@
         <v>27</v>
       </c>
       <c r="B10" t="n">
-        <v>0.049050412637938</v>
+        <v>0.0396943543195528</v>
       </c>
       <c r="C10" t="n">
-        <v>0.298583494433472</v>
+        <v>0.289132376877701</v>
       </c>
       <c r="D10" t="n">
-        <v>0.173816953535705</v>
+        <v>0.164413365598627</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
@@ -1109,13 +1109,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0654657339104391</v>
+        <v>0.0952628451618303</v>
       </c>
       <c r="C11" t="n">
-        <v>0.36429529216567</v>
+        <v>0.412193886231662</v>
       </c>
       <c r="D11" t="n">
-        <v>0.214880513038054</v>
+        <v>0.253728365696746</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
@@ -1126,13 +1126,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0836029492781559</v>
+        <v>0.116719389489182</v>
       </c>
       <c r="C12" t="n">
-        <v>0.358772393594215</v>
+        <v>0.411670310697852</v>
       </c>
       <c r="D12" t="n">
-        <v>0.221187671436185</v>
+        <v>0.264194850093517</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -1143,13 +1143,13 @@
         <v>27</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0515766372614611</v>
+        <v>0.0628096520449353</v>
       </c>
       <c r="C13" t="n">
-        <v>0.357655240573497</v>
+        <v>0.399856826680612</v>
       </c>
       <c r="D13" t="n">
-        <v>0.204615938917479</v>
+        <v>0.231333239362774</v>
       </c>
       <c r="E13" t="s">
         <v>21</v>
@@ -1160,13 +1160,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0627571799624126</v>
+        <v>0.0774956805350221</v>
       </c>
       <c r="C14" t="n">
-        <v>0.209171573802048</v>
+        <v>0.211662114577834</v>
       </c>
       <c r="D14" t="n">
-        <v>0.135964376882231</v>
+        <v>0.144578897556428</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
@@ -1177,13 +1177,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0883313212345291</v>
+        <v>0.106213225852818</v>
       </c>
       <c r="C15" t="n">
-        <v>0.223122207302459</v>
+        <v>0.226535623341326</v>
       </c>
       <c r="D15" t="n">
-        <v>0.155726764268494</v>
+        <v>0.166374424597072</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
@@ -1194,13 +1194,13 @@
         <v>27</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0678552224499854</v>
+        <v>0.0764858670750393</v>
       </c>
       <c r="C16" t="n">
-        <v>0.207290432400413</v>
+        <v>0.202540152645968</v>
       </c>
       <c r="D16" t="n">
-        <v>0.137572827425199</v>
+        <v>0.139513009860504</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
updated paths for results
</commit_message>
<xml_diff>
--- a/results/full_results.xlsx
+++ b/results/full_results.xlsx
@@ -75,7 +75,7 @@
     <t xml:space="preserve">occupation</t>
   </si>
   <si>
-    <t xml:space="preserve">income_hh</t>
+    <t xml:space="preserve">income</t>
   </si>
   <si>
     <t xml:space="preserve">wealth</t>
@@ -502,13 +502,13 @@
         <v>0.306030320695031</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0140135097358763</v>
+        <v>0.0140135097403642</v>
       </c>
       <c r="M2" t="n">
-        <v>0.044042949480424</v>
+        <v>0.0440429494849118</v>
       </c>
       <c r="N2" t="n">
-        <v>0.320043830430907</v>
+        <v>0.320043830435395</v>
       </c>
       <c r="O2"/>
     </row>
@@ -550,10 +550,10 @@
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4" t="n">
-        <v>0.602270479274433</v>
+        <v>0.602270479269944</v>
       </c>
       <c r="I4" t="n">
-        <v>0.285664744666187</v>
+        <v>0.285664744672762</v>
       </c>
       <c r="J4"/>
       <c r="K4"/>
@@ -561,7 +561,7 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4" t="n">
-        <v>0.39786482058513</v>
+        <v>0.397864820589618</v>
       </c>
     </row>
     <row r="5">
@@ -591,13 +591,13 @@
         <v>0.124661493700764</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0258778380079757</v>
+        <v>0.0258778380577954</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0575515385189966</v>
+        <v>0.0575515385688163</v>
       </c>
       <c r="N5" t="n">
-        <v>0.15053933170874</v>
+        <v>0.150539331758559</v>
       </c>
       <c r="O5"/>
     </row>
@@ -639,10 +639,10 @@
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="n">
-        <v>0.819804882768865</v>
+        <v>0.819804882719041</v>
       </c>
       <c r="I7" t="n">
-        <v>0.125102165595073</v>
+        <v>0.125102165652733</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -650,7 +650,7 @@
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7" t="n">
-        <v>0.180258984559252</v>
+        <v>0.180258984609072</v>
       </c>
     </row>
     <row r="8">
@@ -680,13 +680,13 @@
         <v>0.155149501851177</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0418768879942465</v>
+        <v>0.0418768880182208</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0497546069970125</v>
+        <v>0.0497546070209868</v>
       </c>
       <c r="N8" t="n">
-        <v>0.197026389845424</v>
+        <v>0.197026389869398</v>
       </c>
       <c r="O8"/>
     </row>
@@ -728,10 +728,10 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" t="n">
-        <v>0.785914068214634</v>
+        <v>0.785914068190657</v>
       </c>
       <c r="I10" t="n">
-        <v>0.129262717242758</v>
+        <v>0.129262717270778</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
@@ -739,7 +739,7 @@
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10" t="n">
-        <v>0.21416797259564</v>
+        <v>0.214167972619614</v>
       </c>
     </row>
     <row r="11">
@@ -769,13 +769,13 @@
         <v>0.225387262095531</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0283411036012153</v>
+        <v>0.0283411036041199</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0328616107307432</v>
+        <v>0.0328616107336478</v>
       </c>
       <c r="N11" t="n">
-        <v>0.253728365696746</v>
+        <v>0.253728365699651</v>
       </c>
       <c r="O11"/>
     </row>
@@ -817,10 +817,10 @@
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13" t="n">
-        <v>0.73591323923548</v>
+        <v>0.735913239232575</v>
       </c>
       <c r="I13" t="n">
-        <v>0.220052021730966</v>
+        <v>0.220052021734735</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -828,7 +828,7 @@
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13" t="n">
-        <v>0.264194850093517</v>
+        <v>0.264194850096421</v>
       </c>
     </row>
     <row r="14">
@@ -956,13 +956,13 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.258402143126609</v>
+        <v>0.270173855721891</v>
       </c>
       <c r="C2" t="n">
-        <v>0.381685517735206</v>
+        <v>0.369913805148899</v>
       </c>
       <c r="D2" t="n">
-        <v>0.320043830430907</v>
+        <v>0.320043830435395</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -973,13 +973,13 @@
         <v>14</v>
       </c>
       <c r="B3" t="n">
-        <v>0.350235918909555</v>
+        <v>0.356556663617972</v>
       </c>
       <c r="C3" t="n">
-        <v>0.445493722260706</v>
+        <v>0.439172977561264</v>
       </c>
       <c r="D3" t="n">
-        <v>0.39786482058513</v>
+        <v>0.397864820589618</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -990,10 +990,10 @@
         <v>27</v>
       </c>
       <c r="B4" t="n">
-        <v>0.302156483748208</v>
+        <v>0.308862869302389</v>
       </c>
       <c r="C4" t="n">
-        <v>0.405487258461205</v>
+        <v>0.398780872907023</v>
       </c>
       <c r="D4" t="n">
         <v>0.353821871104706</v>
@@ -1007,13 +1007,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0803137283705362</v>
+        <v>0.0869753789565366</v>
       </c>
       <c r="C5" t="n">
-        <v>0.220764935046943</v>
+        <v>0.214103284560582</v>
       </c>
       <c r="D5" t="n">
-        <v>0.15053933170874</v>
+        <v>0.150539331758559</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -1024,13 +1024,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>0.118786280157073</v>
+        <v>0.125933173247459</v>
       </c>
       <c r="C6" t="n">
-        <v>0.241731688961431</v>
+        <v>0.234584795970684</v>
       </c>
       <c r="D6" t="n">
-        <v>0.180258984559252</v>
+        <v>0.180258984609072</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -1041,10 +1041,10 @@
         <v>27</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0639261260280642</v>
+        <v>0.0692263519047685</v>
       </c>
       <c r="C7" t="n">
-        <v>0.181488766052447</v>
+        <v>0.176188540175742</v>
       </c>
       <c r="D7" t="n">
         <v>0.122707446040255</v>
@@ -1058,13 +1058,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0850071193212848</v>
+        <v>0.0771328980096298</v>
       </c>
       <c r="C8" t="n">
-        <v>0.309045660369563</v>
+        <v>0.316919881729166</v>
       </c>
       <c r="D8" t="n">
-        <v>0.197026389845424</v>
+        <v>0.197026389869398</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -1075,13 +1075,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>0.110050467661553</v>
+        <v>0.100892028059918</v>
       </c>
       <c r="C9" t="n">
-        <v>0.318285477529726</v>
+        <v>0.32744391717931</v>
       </c>
       <c r="D9" t="n">
-        <v>0.21416797259564</v>
+        <v>0.214167972619614</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
@@ -1092,10 +1092,10 @@
         <v>27</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0396943543195528</v>
+        <v>0.0341328586480976</v>
       </c>
       <c r="C10" t="n">
-        <v>0.289132376877701</v>
+        <v>0.294693872549156</v>
       </c>
       <c r="D10" t="n">
         <v>0.164413365598627</v>
@@ -1109,13 +1109,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0952628451618303</v>
+        <v>0.0867093433616834</v>
       </c>
       <c r="C11" t="n">
-        <v>0.412193886231662</v>
+        <v>0.420747388037619</v>
       </c>
       <c r="D11" t="n">
-        <v>0.253728365696746</v>
+        <v>0.253728365699651</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
@@ -1126,13 +1126,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.116719389489182</v>
+        <v>0.110305346420244</v>
       </c>
       <c r="C12" t="n">
-        <v>0.411670310697852</v>
+        <v>0.418084353772599</v>
       </c>
       <c r="D12" t="n">
-        <v>0.264194850093517</v>
+        <v>0.264194850096421</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -1143,10 +1143,10 @@
         <v>27</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0628096520449353</v>
+        <v>0.0556392793389844</v>
       </c>
       <c r="C13" t="n">
-        <v>0.399856826680612</v>
+        <v>0.407027199386563</v>
       </c>
       <c r="D13" t="n">
         <v>0.231333239362774</v>
@@ -1160,10 +1160,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0774956805350221</v>
+        <v>0.0759450637572911</v>
       </c>
       <c r="C14" t="n">
-        <v>0.211662114577834</v>
+        <v>0.213212731355565</v>
       </c>
       <c r="D14" t="n">
         <v>0.144578897556428</v>
@@ -1177,10 +1177,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.106213225852818</v>
+        <v>0.103132067181238</v>
       </c>
       <c r="C15" t="n">
-        <v>0.226535623341326</v>
+        <v>0.229616782012906</v>
       </c>
       <c r="D15" t="n">
         <v>0.166374424597072</v>
@@ -1194,10 +1194,10 @@
         <v>27</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0764858670750393</v>
+        <v>0.0725894010190001</v>
       </c>
       <c r="C16" t="n">
-        <v>0.202540152645968</v>
+        <v>0.206436618702007</v>
       </c>
       <c r="D16" t="n">
         <v>0.139513009860504</v>

</xml_diff>

<commit_message>
actually removed math eam pgi
</commit_message>
<xml_diff>
--- a/results/full_results.xlsx
+++ b/results/full_results.xlsx
@@ -499,16 +499,16 @@
         <v>0.353821871104706</v>
       </c>
       <c r="K2" t="n">
-        <v>0.306030320695031</v>
+        <v>0.30548131530695</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0140135097403642</v>
+        <v>0.0151543214118822</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0440429494849118</v>
+        <v>0.0429552022729067</v>
       </c>
       <c r="N2" t="n">
-        <v>0.320043830435395</v>
+        <v>0.320635636718833</v>
       </c>
       <c r="O2"/>
     </row>
@@ -523,10 +523,10 @@
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3" t="n">
-        <v>0.61628713784792</v>
+        <v>0.618516197488937</v>
       </c>
       <c r="G3" t="n">
-        <v>0.306099085751164</v>
+        <v>0.305549957001496</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -550,10 +550,10 @@
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4" t="n">
-        <v>0.602270479269944</v>
+        <v>0.603358470898901</v>
       </c>
       <c r="I4" t="n">
-        <v>0.285664744672762</v>
+        <v>0.283583444307945</v>
       </c>
       <c r="J4"/>
       <c r="K4"/>
@@ -561,7 +561,7 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4" t="n">
-        <v>0.397864820589618</v>
+        <v>0.396777073377613</v>
       </c>
     </row>
     <row r="5">
@@ -588,16 +588,16 @@
         <v>0.122707446040255</v>
       </c>
       <c r="K5" t="n">
-        <v>0.124661493700764</v>
+        <v>0.118711403056588</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0258778380577954</v>
+        <v>0.0284234699386578</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0575515385688163</v>
+        <v>0.0518744755734492</v>
       </c>
       <c r="N5" t="n">
-        <v>0.150539331758559</v>
+        <v>0.147134872995246</v>
       </c>
       <c r="O5"/>
     </row>
@@ -612,10 +612,10 @@
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6" t="n">
-        <v>0.845684736960415</v>
+        <v>0.853908072479899</v>
       </c>
       <c r="G6" t="n">
-        <v>0.124671206276287</v>
+        <v>0.118720652051072</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -639,10 +639,10 @@
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="n">
-        <v>0.819804882719041</v>
+        <v>0.825482388023428</v>
       </c>
       <c r="I7" t="n">
-        <v>0.125102165652733</v>
+        <v>0.120961054165269</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -650,7 +650,7 @@
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7" t="n">
-        <v>0.180258984609072</v>
+        <v>0.174581921613705</v>
       </c>
     </row>
     <row r="8">
@@ -677,16 +677,16 @@
         <v>0.164413365598627</v>
       </c>
       <c r="K8" t="n">
-        <v>0.155149501851177</v>
+        <v>0.154950487430902</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0418768880182208</v>
+        <v>0.0462753967250775</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0497546070209868</v>
+        <v>0.0538964409094861</v>
       </c>
       <c r="N8" t="n">
-        <v>0.197026389869398</v>
+        <v>0.20122588415598</v>
       </c>
       <c r="O8"/>
     </row>
@@ -701,10 +701,10 @@
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9" t="n">
-        <v>0.827795328153142</v>
+        <v>0.828052029768333</v>
       </c>
       <c r="G9" t="n">
-        <v>0.15516569944863</v>
+        <v>0.154966664251263</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -728,10 +728,10 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" t="n">
-        <v>0.785914068190657</v>
+        <v>0.781771801894982</v>
       </c>
       <c r="I10" t="n">
-        <v>0.129262717270778</v>
+        <v>0.130343263131413</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
@@ -739,7 +739,7 @@
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10" t="n">
-        <v>0.214167972619614</v>
+        <v>0.218309806508113</v>
       </c>
     </row>
     <row r="11">
@@ -766,16 +766,16 @@
         <v>0.231333239362774</v>
       </c>
       <c r="K11" t="n">
-        <v>0.225387262095531</v>
+        <v>0.227628738047098</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0283411036041199</v>
+        <v>0.0295879891141118</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0328616107336478</v>
+        <v>0.0375757067530702</v>
       </c>
       <c r="N11" t="n">
-        <v>0.253728365699651</v>
+        <v>0.257216727161209</v>
       </c>
       <c r="O11"/>
     </row>
@@ -790,10 +790,10 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12" t="n">
-        <v>0.764258506127577</v>
+        <v>0.760790786287031</v>
       </c>
       <c r="G12" t="n">
-        <v>0.22542037134725</v>
+        <v>0.22766217657027</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
@@ -817,10 +817,10 @@
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13" t="n">
-        <v>0.735913239232575</v>
+        <v>0.731198450715314</v>
       </c>
       <c r="I13" t="n">
-        <v>0.220052021734735</v>
+        <v>0.222597183806778</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -828,7 +828,7 @@
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13" t="n">
-        <v>0.264194850096421</v>
+        <v>0.268908946115844</v>
       </c>
     </row>
     <row r="14">
@@ -855,16 +855,16 @@
         <v>0.139513009860504</v>
       </c>
       <c r="K14" t="n">
-        <v>0.12889266239111</v>
+        <v>0.129157393728923</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0156862351653176</v>
+        <v>0.0112827630153931</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0268614147365685</v>
+        <v>0.0234822053534689</v>
       </c>
       <c r="N14" t="n">
-        <v>0.144578897556428</v>
+        <v>0.140440156744316</v>
       </c>
       <c r="O14"/>
     </row>
@@ -879,10 +879,10 @@
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15" t="n">
-        <v>0.849387022438783</v>
+        <v>0.848362668967087</v>
       </c>
       <c r="G15" t="n">
-        <v>0.128904076642174</v>
+        <v>0.129168831423602</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -906,10 +906,10 @@
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16" t="n">
-        <v>0.833699398159275</v>
+        <v>0.837078906792492</v>
       </c>
       <c r="I16" t="n">
-        <v>0.140850119093156</v>
+        <v>0.135432813955002</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
@@ -917,7 +917,7 @@
       <c r="M16"/>
       <c r="N16"/>
       <c r="O16" t="n">
-        <v>0.166374424597072</v>
+        <v>0.162995215213972</v>
       </c>
     </row>
   </sheetData>
@@ -956,13 +956,13 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.270173855721891</v>
+        <v>0.268541991328053</v>
       </c>
       <c r="C2" t="n">
-        <v>0.369913805148899</v>
+        <v>0.372729282109613</v>
       </c>
       <c r="D2" t="n">
-        <v>0.320043830435395</v>
+        <v>0.320635636718833</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -973,13 +973,13 @@
         <v>14</v>
       </c>
       <c r="B3" t="n">
-        <v>0.356556663617972</v>
+        <v>0.350898215188114</v>
       </c>
       <c r="C3" t="n">
-        <v>0.439172977561264</v>
+        <v>0.442655931567112</v>
       </c>
       <c r="D3" t="n">
-        <v>0.397864820589618</v>
+        <v>0.396777073377613</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -990,10 +990,10 @@
         <v>27</v>
       </c>
       <c r="B4" t="n">
-        <v>0.308862869302389</v>
+        <v>0.308550083518096</v>
       </c>
       <c r="C4" t="n">
-        <v>0.398780872907023</v>
+        <v>0.399093658691316</v>
       </c>
       <c r="D4" t="n">
         <v>0.353821871104706</v>
@@ -1007,13 +1007,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0869753789565366</v>
+        <v>0.0917942259200481</v>
       </c>
       <c r="C5" t="n">
-        <v>0.214103284560582</v>
+        <v>0.202475520070444</v>
       </c>
       <c r="D5" t="n">
-        <v>0.150539331758559</v>
+        <v>0.147134872995246</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -1024,13 +1024,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>0.125933173247459</v>
+        <v>0.12393792036737</v>
       </c>
       <c r="C6" t="n">
-        <v>0.234584795970684</v>
+        <v>0.225225922860039</v>
       </c>
       <c r="D6" t="n">
-        <v>0.180258984609072</v>
+        <v>0.174581921613705</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -1041,10 +1041,10 @@
         <v>27</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0692263519047685</v>
+        <v>0.0691131899280597</v>
       </c>
       <c r="C7" t="n">
-        <v>0.176188540175742</v>
+        <v>0.176301702152451</v>
       </c>
       <c r="D7" t="n">
         <v>0.122707446040255</v>
@@ -1058,13 +1058,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0771328980096298</v>
+        <v>0.083920337627273</v>
       </c>
       <c r="C8" t="n">
-        <v>0.316919881729166</v>
+        <v>0.318531430684686</v>
       </c>
       <c r="D8" t="n">
-        <v>0.197026389869398</v>
+        <v>0.20122588415598</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -1075,13 +1075,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>0.100892028059918</v>
+        <v>0.106907985058182</v>
       </c>
       <c r="C9" t="n">
-        <v>0.32744391717931</v>
+        <v>0.329711627958044</v>
       </c>
       <c r="D9" t="n">
-        <v>0.214167972619614</v>
+        <v>0.218309806508113</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
@@ -1092,10 +1092,10 @@
         <v>27</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0341328586480976</v>
+        <v>0.0385390742663888</v>
       </c>
       <c r="C10" t="n">
-        <v>0.294693872549156</v>
+        <v>0.290287656930865</v>
       </c>
       <c r="D10" t="n">
         <v>0.164413365598627</v>
@@ -1109,13 +1109,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0867093433616834</v>
+        <v>0.120416345403155</v>
       </c>
       <c r="C11" t="n">
-        <v>0.420747388037619</v>
+        <v>0.394017108919264</v>
       </c>
       <c r="D11" t="n">
-        <v>0.253728365699651</v>
+        <v>0.257216727161209</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
@@ -1126,13 +1126,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.110305346420244</v>
+        <v>0.138419689548485</v>
       </c>
       <c r="C12" t="n">
-        <v>0.418084353772599</v>
+        <v>0.399398202683203</v>
       </c>
       <c r="D12" t="n">
-        <v>0.264194850096421</v>
+        <v>0.268908946115844</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -1143,10 +1143,10 @@
         <v>27</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0556392793389844</v>
+        <v>0.0768065018400139</v>
       </c>
       <c r="C13" t="n">
-        <v>0.407027199386563</v>
+        <v>0.385859976885533</v>
       </c>
       <c r="D13" t="n">
         <v>0.231333239362774</v>
@@ -1160,13 +1160,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0759450637572911</v>
+        <v>0.067715078846633</v>
       </c>
       <c r="C14" t="n">
-        <v>0.213212731355565</v>
+        <v>0.213165234642</v>
       </c>
       <c r="D14" t="n">
-        <v>0.144578897556428</v>
+        <v>0.140440156744316</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
@@ -1177,13 +1177,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.103132067181238</v>
+        <v>0.0925238746145066</v>
       </c>
       <c r="C15" t="n">
-        <v>0.229616782012906</v>
+        <v>0.233466555813438</v>
       </c>
       <c r="D15" t="n">
-        <v>0.166374424597072</v>
+        <v>0.162995215213972</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
@@ -1194,10 +1194,10 @@
         <v>27</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0725894010190001</v>
+        <v>0.0663190443846013</v>
       </c>
       <c r="C16" t="n">
-        <v>0.206436618702007</v>
+        <v>0.212706975336406</v>
       </c>
       <c r="D16" t="n">
         <v>0.139513009860504</v>

</xml_diff>